<commit_message>
refactor: Simplificar importación con estructura Excel sin headers duplicados
- Actualizar ExcelImportService para usar headers únicos
- Revertir readExcelRows a versión simple
- Remover debug code del import wizard
- Nueva estructura: Proyecto ID | Cliente | Proyecto Descripción | FAT | PEM
</commit_message>
<xml_diff>
--- a/doc/excel pruebas/proyectos/Proyectos Automatización.xlsx
+++ b/doc/excel pruebas/proyectos/Proyectos Automatización.xlsx
@@ -9,8 +9,7 @@
   <sheets>
     <sheet name="Proyectos Automatización" sheetId="13" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>Cliente</t>
   </si>
   <si>
-    <t>Proyecto</t>
-  </si>
-  <si>
     <t>CICON SRL</t>
   </si>
   <si>
@@ -59,13 +55,20 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Proyecto ID</t>
+  </si>
+  <si>
+    <t>Proyecto Descripción</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,27 +76,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,15 +97,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -391,7 +374,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -402,7 +385,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -412,21 +395,21 @@
     <col min="3" max="3" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -434,16 +417,16 @@
         <v>3503</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -451,16 +434,16 @@
         <v>3405</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -468,16 +451,16 @@
         <v>3479</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -485,16 +468,16 @@
         <v>3480</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -502,16 +485,16 @@
         <v>3530</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Implementación final módulo Proyectos Automatización (Logs limpios, Docs actualizados)
</commit_message>
<xml_diff>
--- a/doc/excel pruebas/proyectos/Proyectos Automatización.xlsx
+++ b/doc/excel pruebas/proyectos/Proyectos Automatización.xlsx
@@ -57,11 +57,10 @@
     <t>NO</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Proyecto ID</t>
-  </si>
-  <si>
     <t>Proyecto Descripción</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Proyecto ID</t>
   </si>
 </sst>
 </file>
@@ -374,7 +373,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -385,7 +384,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -397,13 +396,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>

</xml_diff>